<commit_message>
deleted patrick's dumb idea
</commit_message>
<xml_diff>
--- a/Final Project/Bill of Materials Final Project.xlsx
+++ b/Final Project/Bill of Materials Final Project.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castia\Documents\GitHub\ee478\Final Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="10035"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -453,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,7 +493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,7 +705,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>